<commit_message>
drop duplicate names, keep row indices when dropping non-gmails
</commit_message>
<xml_diff>
--- a/Testers Virtual Visitas (Responses).xlsx
+++ b/Testers Virtual Visitas (Responses).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/azhang344_gatech_edu/Documents/GitHub/VirtualVisitas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkzr3\VirtualVisitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{E7A59794-3C23-43B4-B843-F6F89FE9904D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F1E968C-6053-4466-AEFF-35F28A59A527}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22368" windowHeight="8196"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -28,9 +27,6 @@
     <t>Email Address</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>From</t>
   </si>
   <si>
@@ -245,12 +241,15 @@
   </si>
   <si>
     <t>Rock, Metal</t>
+  </si>
+  <si>
+    <t>Full Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -526,7 +525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -534,17 +533,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="22" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="22" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,49 +551,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>43896.790636574071</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -602,22 +601,22 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>43896.791250000002</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -625,22 +624,22 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>43896.797939814816</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -648,22 +647,22 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>43896.80159722222</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -671,22 +670,22 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>43896.80201388889</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -694,22 +693,22 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>43896.810069444444</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -717,22 +716,22 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>43896.821539351855</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -740,22 +739,22 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>43896.830578703702</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -763,22 +762,22 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>43897.005486111113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -786,254 +785,254 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>43897.375833333332</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>43901.967476851853</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>43901.967557870368</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>43901.968171296299</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="K14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>43901.968287037038</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>43901.969513888886</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>43901.983182870368</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>